<commit_message>
project description - character profiles
</commit_message>
<xml_diff>
--- a/crew manifest.xlsx
+++ b/crew manifest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\modro\assignment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162C0E11-82D3-4E26-85E8-2A20879D0558}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BB3C36-2007-47F5-9E9B-26AEED6A36CB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1637,7 +1637,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{92B3D360-4624-4115-94D5-4B68FCACB4DD}" name="Table2" displayName="Table2" ref="A1:O289" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:O289" xr:uid="{1BFA0AAA-F1AD-46FE-90F5-135B84BFF5AE}"/>
+  <autoFilter ref="A1:O289" xr:uid="{1BFA0AAA-F1AD-46FE-90F5-135B84BFF5AE}">
+    <filterColumn colId="10">
+      <filters>
+        <filter val="Wouter Loos"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O289">
     <sortCondition ref="N1:N289"/>
   </sortState>
@@ -1961,8 +1967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="I148" sqref="A148:XFD148"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112:XFD112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2031,7 +2037,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -2063,7 +2069,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -2092,7 +2098,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -2127,7 +2133,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -2162,7 +2168,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -2194,7 +2200,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -2226,7 +2232,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -2255,7 +2261,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -2287,7 +2293,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -2316,7 +2322,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -2348,7 +2354,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>73</v>
       </c>
@@ -2371,7 +2377,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>78</v>
       </c>
@@ -2388,7 +2394,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>82</v>
       </c>
@@ -2408,7 +2414,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>85</v>
       </c>
@@ -2434,7 +2440,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>90</v>
       </c>
@@ -2460,7 +2466,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>95</v>
       </c>
@@ -2492,7 +2498,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>102</v>
       </c>
@@ -2518,7 +2524,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>109</v>
       </c>
@@ -2544,7 +2550,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>114</v>
       </c>
@@ -2573,7 +2579,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>119</v>
       </c>
@@ -2593,7 +2599,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>119</v>
       </c>
@@ -2613,7 +2619,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>123</v>
       </c>
@@ -2642,7 +2648,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>127</v>
       </c>
@@ -2674,7 +2680,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>131</v>
       </c>
@@ -2697,7 +2703,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>90</v>
       </c>
@@ -2723,7 +2729,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>136</v>
       </c>
@@ -2749,7 +2755,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>139</v>
       </c>
@@ -2778,7 +2784,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>143</v>
       </c>
@@ -2801,7 +2807,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>146</v>
       </c>
@@ -2830,7 +2836,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>149</v>
       </c>
@@ -2850,7 +2856,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>152</v>
       </c>
@@ -2879,12 +2885,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="N33" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>155</v>
       </c>
@@ -2901,7 +2907,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>157</v>
       </c>
@@ -2921,7 +2927,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>157</v>
       </c>
@@ -2941,7 +2947,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>157</v>
       </c>
@@ -2961,7 +2967,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>157</v>
       </c>
@@ -2981,7 +2987,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>157</v>
       </c>
@@ -3001,7 +3007,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>157</v>
       </c>
@@ -3021,7 +3027,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>157</v>
       </c>
@@ -3041,7 +3047,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>157</v>
       </c>
@@ -3061,7 +3067,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>157</v>
       </c>
@@ -3081,7 +3087,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>157</v>
       </c>
@@ -3101,7 +3107,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>157</v>
       </c>
@@ -3121,7 +3127,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>162</v>
       </c>
@@ -3144,7 +3150,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>90</v>
       </c>
@@ -3173,7 +3179,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>171</v>
       </c>
@@ -3199,7 +3205,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>174</v>
       </c>
@@ -3219,7 +3225,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>24</v>
       </c>
@@ -3248,7 +3254,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>183</v>
       </c>
@@ -3280,7 +3286,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>189</v>
       </c>
@@ -3303,7 +3309,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>194</v>
       </c>
@@ -3332,7 +3338,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>198</v>
       </c>
@@ -3352,7 +3358,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>198</v>
       </c>
@@ -3372,7 +3378,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>198</v>
       </c>
@@ -3392,7 +3398,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>198</v>
       </c>
@@ -3412,7 +3418,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>198</v>
       </c>
@@ -3432,7 +3438,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>198</v>
       </c>
@@ -3452,7 +3458,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>198</v>
       </c>
@@ -3475,7 +3481,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>198</v>
       </c>
@@ -3498,7 +3504,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>198</v>
       </c>
@@ -3515,7 +3521,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>198</v>
       </c>
@@ -3532,7 +3538,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>198</v>
       </c>
@@ -3549,7 +3555,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>198</v>
       </c>
@@ -3566,7 +3572,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>198</v>
       </c>
@@ -3583,7 +3589,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>198</v>
       </c>
@@ -3600,7 +3606,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>95</v>
       </c>
@@ -3629,7 +3635,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>207</v>
       </c>
@@ -3655,7 +3661,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>90</v>
       </c>
@@ -3684,7 +3690,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>215</v>
       </c>
@@ -3704,7 +3710,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>194</v>
       </c>
@@ -3733,7 +3739,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>24</v>
       </c>
@@ -3765,7 +3771,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>227</v>
       </c>
@@ -3791,7 +3797,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>233</v>
       </c>
@@ -3817,7 +3823,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>239</v>
       </c>
@@ -3834,7 +3840,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>242</v>
       </c>
@@ -3857,7 +3863,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>245</v>
       </c>
@@ -3880,7 +3886,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>251</v>
       </c>
@@ -3938,7 +3944,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>183</v>
       </c>
@@ -3967,7 +3973,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>266</v>
       </c>
@@ -4022,7 +4028,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>270</v>
       </c>
@@ -4051,7 +4057,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>274</v>
       </c>
@@ -4077,7 +4083,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>275</v>
       </c>
@@ -4103,7 +4109,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>276</v>
       </c>
@@ -4129,7 +4135,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>278</v>
       </c>
@@ -4155,7 +4161,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>30</v>
       </c>
@@ -4181,7 +4187,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>286</v>
       </c>
@@ -4207,7 +4213,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>183</v>
       </c>
@@ -4236,7 +4242,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>292</v>
       </c>
@@ -4262,7 +4268,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>30</v>
       </c>
@@ -4288,7 +4294,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>73</v>
       </c>
@@ -4302,7 +4308,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>73</v>
       </c>
@@ -4322,7 +4328,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>15</v>
       </c>
@@ -4342,7 +4348,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>24</v>
       </c>
@@ -4365,7 +4371,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>292</v>
       </c>
@@ -4379,7 +4385,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>189</v>
       </c>
@@ -4405,7 +4411,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>189</v>
       </c>
@@ -4416,7 +4422,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>315</v>
       </c>
@@ -4427,7 +4433,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>317</v>
       </c>
@@ -4450,7 +4456,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>198</v>
       </c>
@@ -4467,7 +4473,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>127</v>
       </c>
@@ -4484,7 +4490,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>127</v>
       </c>
@@ -4504,7 +4510,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>127</v>
       </c>
@@ -4518,7 +4524,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>329</v>
       </c>
@@ -4544,7 +4550,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>194</v>
       </c>
@@ -4561,7 +4567,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>194</v>
       </c>
@@ -4575,7 +4581,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>194</v>
       </c>
@@ -4598,7 +4604,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>194</v>
       </c>
@@ -4618,7 +4624,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>194</v>
       </c>
@@ -4644,7 +4650,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>194</v>
       </c>
@@ -4658,7 +4664,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>340</v>
       </c>
@@ -4681,7 +4687,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>342</v>
       </c>
@@ -4707,7 +4713,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>345</v>
       </c>
@@ -4721,7 +4727,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>348</v>
       </c>
@@ -4732,7 +4738,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>350</v>
       </c>
@@ -4752,7 +4758,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>354</v>
       </c>
@@ -4766,7 +4772,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>354</v>
       </c>
@@ -4783,7 +4789,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>359</v>
       </c>
@@ -4794,7 +4800,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>362</v>
       </c>
@@ -4823,7 +4829,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>366</v>
       </c>
@@ -4840,7 +4846,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>85</v>
       </c>
@@ -4860,7 +4866,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>85</v>
       </c>
@@ -4877,7 +4883,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>85</v>
       </c>
@@ -4903,7 +4909,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>374</v>
       </c>
@@ -4917,7 +4923,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>183</v>
       </c>
@@ -4931,7 +4937,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>183</v>
       </c>
@@ -4945,7 +4951,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>380</v>
       </c>
@@ -4965,7 +4971,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>90</v>
       </c>
@@ -4988,7 +4994,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>30</v>
       </c>
@@ -5008,7 +5014,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>30</v>
       </c>
@@ -5034,7 +5040,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>30</v>
       </c>
@@ -5051,7 +5057,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>30</v>
       </c>
@@ -5068,7 +5074,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>30</v>
       </c>
@@ -5082,7 +5088,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>30</v>
       </c>
@@ -5105,7 +5111,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>30</v>
       </c>
@@ -5125,7 +5131,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>402</v>
       </c>
@@ -5145,7 +5151,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>406</v>
       </c>
@@ -5162,7 +5168,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>410</v>
       </c>
@@ -5173,7 +5179,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>410</v>
       </c>
@@ -5187,7 +5193,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>410</v>
       </c>
@@ -5198,7 +5204,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>410</v>
       </c>
@@ -5218,7 +5224,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>410</v>
       </c>
@@ -5244,7 +5250,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>422</v>
       </c>
@@ -5261,7 +5267,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>426</v>
       </c>
@@ -5278,7 +5284,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>427</v>
       </c>
@@ -5292,7 +5298,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>430</v>
       </c>
@@ -5303,7 +5309,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>430</v>
       </c>
@@ -5320,7 +5326,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>430</v>
       </c>
@@ -5331,7 +5337,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>434</v>
       </c>
@@ -5342,7 +5348,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>436</v>
       </c>
@@ -5359,7 +5365,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>440</v>
       </c>
@@ -5370,7 +5376,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>443</v>
       </c>
@@ -5393,7 +5399,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>445</v>
       </c>
@@ -5413,7 +5419,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>448</v>
       </c>
@@ -5433,7 +5439,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>452</v>
       </c>
@@ -5450,7 +5456,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>455</v>
       </c>
@@ -5473,7 +5479,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>459</v>
       </c>
@@ -5490,7 +5496,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>463</v>
       </c>
@@ -5510,7 +5516,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>464</v>
       </c>
@@ -5524,7 +5530,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>67</v>
       </c>
@@ -5535,7 +5541,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>466</v>
       </c>
@@ -5549,7 +5555,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>469</v>
       </c>
@@ -5563,7 +5569,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>471</v>
       </c>
@@ -5577,7 +5583,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>472</v>
       </c>
@@ -5597,7 +5603,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>152</v>
       </c>
@@ -5620,7 +5626,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>477</v>
       </c>
@@ -5634,7 +5640,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>149</v>
       </c>
@@ -5648,6 +5654,125 @@
         <v>480</v>
       </c>
     </row>
+    <row r="171" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="172" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="173" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="174" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="175" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="176" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="177" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="178" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="179" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="180" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="181" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="182" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="183" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="184" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="185" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="186" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="187" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="188" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="189" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="190" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="191" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="192" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="193" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="194" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="195" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="196" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="197" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="198" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="199" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="200" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="201" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="202" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="203" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="204" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="205" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="206" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="207" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="208" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="209" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="210" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="211" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="212" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="213" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="214" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="215" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="216" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="217" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="218" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="219" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="220" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="221" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="222" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="223" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="224" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="225" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="226" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="227" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="228" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="229" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="230" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="231" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="232" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="233" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="234" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="235" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="236" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="237" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="238" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="239" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="240" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="241" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="242" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="243" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="244" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="245" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="246" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="247" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="248" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="249" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="250" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="251" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="252" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="253" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="254" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="255" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="256" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="257" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="258" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="259" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="260" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="261" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="262" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="263" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="264" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="265" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="266" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="267" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="268" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="269" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="270" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="271" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="272" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="273" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="274" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="275" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="276" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="277" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="278" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="279" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="280" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="281" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="282" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="283" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="284" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="285" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="286" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="287" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="288" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="289" spans="1:14" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="290" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>119</v>

</xml_diff>